<commit_message>
Chi vs eta and epsilon for whole Array
added chi relative to G_DN
</commit_message>
<xml_diff>
--- a/Results/06_Jun_15/Chi vs Eta 20 Feb 2015.xlsx
+++ b/Results/06_Jun_15/Chi vs Eta 20 Feb 2015.xlsx
@@ -15,7 +15,6 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="152511"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -3617,11 +3616,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="347427376"/>
-        <c:axId val="347430904"/>
+        <c:axId val="119478672"/>
+        <c:axId val="119479848"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="347427376"/>
+        <c:axId val="119478672"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3720,12 +3719,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="347430904"/>
+        <c:crossAx val="119479848"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="347430904"/>
+        <c:axId val="119479848"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3838,7 +3837,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="347427376"/>
+        <c:crossAx val="119478672"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4744,7 +4743,7 @@
   <dimension ref="A1:F553"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="W14" sqref="W14"/>
+      <selection activeCell="W12" sqref="W12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9184,6 +9183,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>